<commit_message>
- la pornirea aplicatiei, suntem atentionati despre evenimentele periodice - am adaugat tutorialul sub forma .html
</commit_message>
<xml_diff>
--- a/Gestiune Cheltuieli/bin/Debug/raport.xlsx
+++ b/Gestiune Cheltuieli/bin/Debug/raport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Data</t>
   </si>
@@ -48,10 +48,16 @@
     <t>Plata factura curent</t>
   </si>
   <si>
+    <t>saptamanal</t>
+  </si>
+  <si>
     <t>Am cumparat un frigider</t>
   </si>
   <si>
     <t>Am primit datoria de la X</t>
+  </si>
+  <si>
+    <t>Factura</t>
   </si>
 </sst>
 </file>
@@ -408,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -483,7 +489,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>155</v>
@@ -494,7 +500,7 @@
         <v>41013.97284722222</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -508,13 +514,27 @@
         <v>41014.975405092591</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7">
         <v>1300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>41010.710532407407</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tratat 'Inapoi' pe "Adauga eveniment" si "Modifica eveniment"
</commit_message>
<xml_diff>
--- a/Gestiune Cheltuieli/bin/Debug/raport.xlsx
+++ b/Gestiune Cheltuieli/bin/Debug/raport.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="21075" windowHeight="12075"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="19155" windowHeight="11055"/>
   </bookViews>
   <sheets>
     <sheet name="Cheltuieli si venituri" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Data</t>
   </si>
@@ -30,46 +30,71 @@
     <t>Suma</t>
   </si>
   <si>
+    <t>11.04.2012 23:23:59</t>
+  </si>
+  <si>
     <t>Am castigat la loto</t>
   </si>
   <si>
     <t xml:space="preserve"> - </t>
   </si>
   <si>
+    <t>12.04.2012 23:20:02</t>
+  </si>
+  <si>
     <t>Salariu</t>
   </si>
   <si>
     <t>lunar</t>
   </si>
   <si>
+    <t>02.04.2012 23:30:49</t>
+  </si>
+  <si>
     <t>Am pierdut niste bani</t>
   </si>
   <si>
+    <t>11.04.2012 23:20:22</t>
+  </si>
+  <si>
     <t>Plata factura curent</t>
   </si>
   <si>
     <t>saptamanal</t>
   </si>
   <si>
+    <t>08.04.2012 23:20:54</t>
+  </si>
+  <si>
     <t>Am cumparat un frigider</t>
   </si>
   <si>
+    <t>10.04.2012 23:24:35</t>
+  </si>
+  <si>
     <t>Am primit datoria de la X</t>
   </si>
   <si>
-    <t>Factura</t>
+    <t>11.04.2012 17:03:10</t>
+  </si>
+  <si>
+    <t>Factura2</t>
+  </si>
+  <si>
+    <t>09.04.2012 18:01:09</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -78,6 +103,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -103,14 +129,11 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -118,12 +141,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -202,7 +220,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -237,7 +254,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,19 +429,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="64.7109375" customWidth="1"/>
     <col min="3" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,129 +455,143 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>41010.974988425929</v>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>41011.972245370373</v>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>2200</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>41011.979733796295</v>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>41012.97247685185</v>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>41013.97284722222</v>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>570</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>41014.975405092591</v>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>1300</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>41010.710532407407</v>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>100</v>
       </c>
     </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>